<commit_message>
Small correction in training clasification
</commit_message>
<xml_diff>
--- a/Review files/qald9_train_set_review_table.xlsx
+++ b/Review files/qald9_train_set_review_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javi\Desktop\Work\QALD9ES\Repo\QALD9-ES\Review files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CDBA4D-E156-4C1F-8B78-D1D6F7174FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B565CC-14B0-47FF-BDA2-FC2CA68CA151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="1290" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2569" uniqueCount="2176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2572" uniqueCount="2176">
   <si>
     <t>id</t>
   </si>
@@ -6997,10 +6997,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="E151" sqref="E151"/>
+      <selection pane="bottomLeft" activeCell="D152" sqref="D152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8104,6 +8104,9 @@
       <c r="K39" t="s">
         <v>2010</v>
       </c>
+      <c r="N39" t="s">
+        <v>2010</v>
+      </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -8234,6 +8237,9 @@
       <c r="K44" t="s">
         <v>2010</v>
       </c>
+      <c r="N44" t="s">
+        <v>2010</v>
+      </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -8260,6 +8266,9 @@
       <c r="K45" t="s">
         <v>2010</v>
       </c>
+      <c r="N45" t="s">
+        <v>2010</v>
+      </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -11144,9 +11153,10 @@
       <c r="A149" t="s">
         <v>161</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B149" s="2" t="s">
         <v>569</v>
       </c>
+      <c r="C149" s="2"/>
       <c r="D149" t="s">
         <v>2172</v>
       </c>
@@ -15539,6 +15549,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N412">
+    <sortCondition ref="A2:A412"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
85% of the trainset translated
</commit_message>
<xml_diff>
--- a/Review files/qald9_train_set_review_table.xlsx
+++ b/Review files/qald9_train_set_review_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javi\Desktop\Work\QALD9ES\Repo\QALD9-ES\Review files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0FE703-4E22-4E63-9032-9B15187AEEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF9940E-E80B-4E4B-A253-D7040A9A196C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3136" uniqueCount="2365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3339" uniqueCount="2435">
   <si>
     <t>id</t>
   </si>
@@ -7133,6 +7133,216 @@
   </si>
   <si>
     <t>Pink Floyd, The Wall, escritores</t>
+  </si>
+  <si>
+    <t>Australia, ciudad, más grande</t>
+  </si>
+  <si>
+    <t>casado, presidente, Chirac</t>
+  </si>
+  <si>
+    <t>¿Cuál es el sistema de gobierno en Sudáfrica?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sistema de gobierno , Sudáfrica </t>
+  </si>
+  <si>
+    <t>¿Cuál es la altura de la torre marina de Yokohama?</t>
+  </si>
+  <si>
+    <t>altura, torre marina Yokohama</t>
+  </si>
+  <si>
+    <t>¿Qué días festivos son festejados en todo el mundo?</t>
+  </si>
+  <si>
+    <t>días festivos, todo el mundo</t>
+  </si>
+  <si>
+    <t>¿Quién es el jugador de baloncesto más alto?</t>
+  </si>
+  <si>
+    <t>jugador de baloncesto, más alto</t>
+  </si>
+  <si>
+    <t>idiomas, Turkmenistán, cuántos</t>
+  </si>
+  <si>
+    <t>¿Alguna vez ganó Kaurismäki el Gran Prix de Cannes?</t>
+  </si>
+  <si>
+    <t>¿A qué partido político pertenece el alcalde de París?</t>
+  </si>
+  <si>
+    <t>partido político, alcalde, París</t>
+  </si>
+  <si>
+    <t>¿Quién es el conductor de Fórmula 1 con más carreras?</t>
+  </si>
+  <si>
+    <t>conductor, Fórmula 1, carreras, más</t>
+  </si>
+  <si>
+    <t>país, origen, Sitecore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lugar de nacimiento,  Frank Sinatra </t>
+  </si>
+  <si>
+    <t>¿Dónde nació Frank Sinatra?</t>
+  </si>
+  <si>
+    <t>hijo, Sonny, Cher</t>
+  </si>
+  <si>
+    <t>¿Cuántos grupos étnicos hay en Eslovenia?</t>
+  </si>
+  <si>
+    <t>grupos étnicos, Eslovenia</t>
+  </si>
+  <si>
+    <t>¿Nació Natalie Portman en los Estados Unidos de América?</t>
+  </si>
+  <si>
+    <t>Natalie Portman,nacimiento, Estados Unidos de América</t>
+  </si>
+  <si>
+    <t>¿Quién es el hijo mayor de Meryl Streep?</t>
+  </si>
+  <si>
+    <t>hijo, mayor, Meryl Streep</t>
+  </si>
+  <si>
+    <t>¿Qué series de televisión creó Walt Disney?</t>
+  </si>
+  <si>
+    <t>series de televisión, creó, Walt Disney</t>
+  </si>
+  <si>
+    <t>¿Qué tipo de uvas crecen en Oregón?</t>
+  </si>
+  <si>
+    <t>tipo uva, crece, Oregón</t>
+  </si>
+  <si>
+    <t>¿Estuvo el presidente americano Jackson involucrado en una guerra?</t>
+  </si>
+  <si>
+    <t>presidente americano, Jackson, guerra</t>
+  </si>
+  <si>
+    <t>¿Cuándo se completó el Titanic?</t>
+  </si>
+  <si>
+    <t>¿Ganó Tesla el premio nobel de física?</t>
+  </si>
+  <si>
+    <t>¿Cuántos estados tiene México?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estados ,  México </t>
+  </si>
+  <si>
+    <t>¿Qué científico es conocido por haber participado en el proyecto Manhattan y ganar el premio Nobel de la Paz?</t>
+  </si>
+  <si>
+    <t>científico,  proyecto Manhattan, premio Nobel de la Paz</t>
+  </si>
+  <si>
+    <t>¿Cuánto costó la película de Lego?</t>
+  </si>
+  <si>
+    <t>precio, película, Lego</t>
+  </si>
+  <si>
+    <t>serie de televisión, HBO, Los Sopranos, primera temporada, episodios</t>
+  </si>
+  <si>
+    <t>¿Qué ciudad tiene la menor población?</t>
+  </si>
+  <si>
+    <t>ciudad, menor, población</t>
+  </si>
+  <si>
+    <t>ubicación, enterrado, Syngman Rhee</t>
+  </si>
+  <si>
+    <t>¿Neymar juega en el Real Madrid?</t>
+  </si>
+  <si>
+    <t>príncipe Harry, príncipe William, mismos padres</t>
+  </si>
+  <si>
+    <t>¿Tienen el príncipe Harry y el príncipe William los mismos padres?</t>
+  </si>
+  <si>
+    <t>¿Quién fue el supervisor doctoral de Albert Einstein?</t>
+  </si>
+  <si>
+    <t>¿Quién inspiró a Vincent van Gogh?</t>
+  </si>
+  <si>
+    <t>persona, inpiración, Vincent van Gogh</t>
+  </si>
+  <si>
+    <t>¿Qué edificio tiene más pisos luego del Burj Khalifa?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edificio ,  después ,  Burj Khalifa,  más pisos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">resultado ,  Guerra de las Rosas </t>
+  </si>
+  <si>
+    <t>¿Cuál fue el resultado final de la Guerra de las Rosas?</t>
+  </si>
+  <si>
+    <t>¿Cuanto costó Pulp Fiction?</t>
+  </si>
+  <si>
+    <t>costó, Pulp Fiction</t>
+  </si>
+  <si>
+    <t>¿Es la proinsulina una proteína?</t>
+  </si>
+  <si>
+    <t>proinsulina, proteína</t>
+  </si>
+  <si>
+    <t>¿Tienen el Urdu y el Persa una raíz en común?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">urdu ,  persa , raíz en común </t>
+  </si>
+  <si>
+    <t>¿Quién actúa en películas españolas producidas por Benicio del Toro?</t>
+  </si>
+  <si>
+    <t>actores, películas, españolas, productor, Benicio del Toro</t>
+  </si>
+  <si>
+    <t>¿Es el lago Baikal más grande que el Gran Lago del Oso?</t>
+  </si>
+  <si>
+    <t>lago Baikal, más grande, Gran lago del Oso</t>
+  </si>
+  <si>
+    <t>¿Cuáles son los libros de la serie de Fundación de Asimov?</t>
+  </si>
+  <si>
+    <t>libros, serie Fundación, Asimov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ciudad ,  más antiguo, funcional, metro </t>
+  </si>
+  <si>
+    <t>¿Qué ciudad tiene el metro en funcionamiento más antiguo?</t>
+  </si>
+  <si>
+    <t>¿Quién diseñó el puente de Brooklyn?</t>
+  </si>
+  <si>
+    <t>diseñador, puente de Brooklyn</t>
   </si>
 </sst>
 </file>
@@ -7566,9 +7776,9 @@
   <dimension ref="A1:N409"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A276" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A308" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="B297" sqref="B297"/>
+      <selection pane="bottomLeft" activeCell="B347" sqref="B347"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15950,11 +16160,23 @@
       <c r="C297" t="s">
         <v>1113</v>
       </c>
+      <c r="D297" t="s">
+        <v>1113</v>
+      </c>
       <c r="E297" t="s">
         <v>1503</v>
       </c>
       <c r="F297" t="s">
         <v>1898</v>
+      </c>
+      <c r="G297" t="s">
+        <v>2365</v>
+      </c>
+      <c r="K297" t="s">
+        <v>2009</v>
+      </c>
+      <c r="N297" t="s">
+        <v>2009</v>
       </c>
     </row>
     <row r="298" spans="1:14" x14ac:dyDescent="0.25">
@@ -15967,25 +16189,50 @@
       <c r="C298" t="s">
         <v>1114</v>
       </c>
+      <c r="D298" t="s">
+        <v>1114</v>
+      </c>
       <c r="E298" t="s">
         <v>1504</v>
       </c>
       <c r="F298" t="s">
         <v>1899</v>
+      </c>
+      <c r="G298" t="s">
+        <v>2366</v>
+      </c>
+      <c r="K298" t="s">
+        <v>2009</v>
+      </c>
+      <c r="M298" t="s">
+        <v>2009</v>
       </c>
     </row>
     <row r="299" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>311</v>
       </c>
-      <c r="B299" t="s">
+      <c r="B299" s="2" t="s">
         <v>719</v>
+      </c>
+      <c r="C299" s="2"/>
+      <c r="D299" t="s">
+        <v>2367</v>
       </c>
       <c r="E299" t="s">
         <v>1505</v>
       </c>
       <c r="F299" t="s">
         <v>1900</v>
+      </c>
+      <c r="G299" t="s">
+        <v>2368</v>
+      </c>
+      <c r="J299" t="s">
+        <v>2009</v>
+      </c>
+      <c r="K299" t="s">
+        <v>2009</v>
       </c>
     </row>
     <row r="300" spans="1:14" x14ac:dyDescent="0.25">
@@ -15998,22 +16245,50 @@
       <c r="C300" t="s">
         <v>1115</v>
       </c>
+      <c r="D300" t="s">
+        <v>2369</v>
+      </c>
       <c r="E300" t="s">
         <v>1506</v>
       </c>
       <c r="F300" t="s">
         <v>1901</v>
+      </c>
+      <c r="G300" t="s">
+        <v>2370</v>
+      </c>
+      <c r="I300" t="s">
+        <v>2009</v>
+      </c>
+      <c r="K300" t="s">
+        <v>2009</v>
+      </c>
+      <c r="M300" t="s">
+        <v>2009</v>
       </c>
     </row>
     <row r="301" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>313</v>
       </c>
-      <c r="B301" t="s">
+      <c r="B301" s="2" t="s">
         <v>721</v>
+      </c>
+      <c r="C301" s="2"/>
+      <c r="D301" t="s">
+        <v>2371</v>
       </c>
       <c r="E301" t="s">
         <v>1356</v>
+      </c>
+      <c r="G301" t="s">
+        <v>2372</v>
+      </c>
+      <c r="J301" t="s">
+        <v>2009</v>
+      </c>
+      <c r="K301" t="s">
+        <v>2009</v>
       </c>
     </row>
     <row r="302" spans="1:14" x14ac:dyDescent="0.25">
@@ -16026,11 +16301,26 @@
       <c r="C302" t="s">
         <v>1116</v>
       </c>
+      <c r="D302" t="s">
+        <v>2373</v>
+      </c>
       <c r="E302" t="s">
         <v>1507</v>
       </c>
       <c r="F302" t="s">
         <v>1902</v>
+      </c>
+      <c r="G302" t="s">
+        <v>2374</v>
+      </c>
+      <c r="H302" t="s">
+        <v>2009</v>
+      </c>
+      <c r="K302" t="s">
+        <v>2009</v>
+      </c>
+      <c r="L302" t="s">
+        <v>2009</v>
       </c>
     </row>
     <row r="303" spans="1:14" x14ac:dyDescent="0.25">
@@ -16043,11 +16333,23 @@
       <c r="C303" t="s">
         <v>1117</v>
       </c>
+      <c r="D303" t="s">
+        <v>1117</v>
+      </c>
       <c r="E303" t="s">
         <v>1508</v>
       </c>
       <c r="F303" t="s">
         <v>1903</v>
+      </c>
+      <c r="G303" t="s">
+        <v>2375</v>
+      </c>
+      <c r="K303" t="s">
+        <v>2009</v>
+      </c>
+      <c r="N303" t="s">
+        <v>2009</v>
       </c>
     </row>
     <row r="304" spans="1:14" x14ac:dyDescent="0.25">
@@ -16060,14 +16362,23 @@
       <c r="C304" t="s">
         <v>1118</v>
       </c>
+      <c r="D304" t="s">
+        <v>1118</v>
+      </c>
       <c r="E304" t="s">
         <v>1509</v>
       </c>
       <c r="F304" t="s">
         <v>1904</v>
       </c>
-    </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G304" t="s">
+        <v>1904</v>
+      </c>
+      <c r="N304" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="305" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>317</v>
       </c>
@@ -16077,14 +16388,29 @@
       <c r="C305" t="s">
         <v>1119</v>
       </c>
+      <c r="D305" t="s">
+        <v>2376</v>
+      </c>
       <c r="E305" t="s">
         <v>1510</v>
       </c>
       <c r="F305" t="s">
         <v>1905</v>
       </c>
-    </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G305" t="s">
+        <v>1905</v>
+      </c>
+      <c r="I305" t="s">
+        <v>2009</v>
+      </c>
+      <c r="L305" t="s">
+        <v>2009</v>
+      </c>
+      <c r="M305" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="306" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>318</v>
       </c>
@@ -16094,14 +16420,26 @@
       <c r="C306" t="s">
         <v>1120</v>
       </c>
+      <c r="D306" t="s">
+        <v>2377</v>
+      </c>
       <c r="E306" t="s">
         <v>1511</v>
       </c>
       <c r="F306" t="s">
         <v>1906</v>
       </c>
-    </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G306" t="s">
+        <v>2378</v>
+      </c>
+      <c r="K306" t="s">
+        <v>2009</v>
+      </c>
+      <c r="L306" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="307" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>319</v>
       </c>
@@ -16111,14 +16449,26 @@
       <c r="C307" t="s">
         <v>1121</v>
       </c>
+      <c r="D307" t="s">
+        <v>2379</v>
+      </c>
       <c r="E307" t="s">
         <v>1512</v>
       </c>
       <c r="F307" t="s">
         <v>1907</v>
       </c>
-    </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G307" t="s">
+        <v>2380</v>
+      </c>
+      <c r="K307" t="s">
+        <v>2009</v>
+      </c>
+      <c r="L307" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="308" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>320</v>
       </c>
@@ -16128,19 +16478,35 @@
       <c r="C308" t="s">
         <v>1122</v>
       </c>
+      <c r="D308" t="s">
+        <v>1122</v>
+      </c>
       <c r="E308" t="s">
         <v>1513</v>
       </c>
       <c r="F308" t="s">
         <v>1908</v>
       </c>
-    </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G308" t="s">
+        <v>2381</v>
+      </c>
+      <c r="K308" t="s">
+        <v>2009</v>
+      </c>
+      <c r="N308" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="309" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>321</v>
       </c>
-      <c r="B309" t="s">
+      <c r="B309" s="2" t="s">
         <v>729</v>
+      </c>
+      <c r="C309" s="2"/>
+      <c r="D309" t="s">
+        <v>2383</v>
       </c>
       <c r="E309" t="s">
         <v>1514</v>
@@ -16148,8 +16514,20 @@
       <c r="F309" t="s">
         <v>1909</v>
       </c>
-    </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G309" t="s">
+        <v>2382</v>
+      </c>
+      <c r="I309" t="s">
+        <v>2009</v>
+      </c>
+      <c r="J309" t="s">
+        <v>2009</v>
+      </c>
+      <c r="K309" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="310" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>322</v>
       </c>
@@ -16159,14 +16537,23 @@
       <c r="C310" t="s">
         <v>1123</v>
       </c>
+      <c r="D310" t="s">
+        <v>1123</v>
+      </c>
       <c r="E310" t="s">
         <v>1515</v>
       </c>
       <c r="F310" t="s">
         <v>1910</v>
       </c>
-    </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G310" t="s">
+        <v>1910</v>
+      </c>
+      <c r="N310" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="311" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>323</v>
       </c>
@@ -16176,14 +16563,26 @@
       <c r="C311" t="s">
         <v>1124</v>
       </c>
+      <c r="D311" t="s">
+        <v>1124</v>
+      </c>
       <c r="E311" t="s">
         <v>1516</v>
       </c>
       <c r="F311" t="s">
         <v>1911</v>
       </c>
-    </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G311" t="s">
+        <v>2384</v>
+      </c>
+      <c r="K311" t="s">
+        <v>2009</v>
+      </c>
+      <c r="N311" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="312" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>324</v>
       </c>
@@ -16193,14 +16592,26 @@
       <c r="C312" t="s">
         <v>1125</v>
       </c>
+      <c r="D312" t="s">
+        <v>2385</v>
+      </c>
       <c r="E312" t="s">
         <v>1517</v>
       </c>
       <c r="F312" t="s">
         <v>1912</v>
       </c>
-    </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G312" t="s">
+        <v>2386</v>
+      </c>
+      <c r="K312" t="s">
+        <v>2009</v>
+      </c>
+      <c r="M312" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="313" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>325</v>
       </c>
@@ -16210,14 +16621,23 @@
       <c r="C313" t="s">
         <v>1126</v>
       </c>
+      <c r="D313" t="s">
+        <v>1126</v>
+      </c>
       <c r="E313" t="s">
         <v>1518</v>
       </c>
       <c r="F313" t="s">
         <v>1913</v>
       </c>
-    </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G313" t="s">
+        <v>1913</v>
+      </c>
+      <c r="N313" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="314" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>326</v>
       </c>
@@ -16227,14 +16647,26 @@
       <c r="C314" t="s">
         <v>1127</v>
       </c>
+      <c r="D314" t="s">
+        <v>2387</v>
+      </c>
       <c r="E314" t="s">
         <v>1519</v>
       </c>
       <c r="F314" t="s">
         <v>1914</v>
       </c>
-    </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G314" t="s">
+        <v>2388</v>
+      </c>
+      <c r="H314" t="s">
+        <v>2009</v>
+      </c>
+      <c r="K314" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="315" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>327</v>
       </c>
@@ -16244,14 +16676,23 @@
       <c r="C315" t="s">
         <v>1128</v>
       </c>
+      <c r="D315" t="s">
+        <v>1128</v>
+      </c>
       <c r="E315" t="s">
         <v>1520</v>
       </c>
       <c r="F315" t="s">
         <v>1915</v>
       </c>
-    </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G315" t="s">
+        <v>1915</v>
+      </c>
+      <c r="N315" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="316" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>328</v>
       </c>
@@ -16261,14 +16702,32 @@
       <c r="C316" t="s">
         <v>1129</v>
       </c>
+      <c r="D316" t="s">
+        <v>2389</v>
+      </c>
       <c r="E316" t="s">
         <v>1521</v>
       </c>
       <c r="F316" t="s">
         <v>1916</v>
       </c>
-    </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G316" t="s">
+        <v>2390</v>
+      </c>
+      <c r="H316" t="s">
+        <v>2009</v>
+      </c>
+      <c r="K316" t="s">
+        <v>2009</v>
+      </c>
+      <c r="L316" t="s">
+        <v>2009</v>
+      </c>
+      <c r="M316" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="317" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>329</v>
       </c>
@@ -16278,14 +16737,26 @@
       <c r="C317" t="s">
         <v>1130</v>
       </c>
+      <c r="D317" t="s">
+        <v>2391</v>
+      </c>
       <c r="E317" t="s">
         <v>1522</v>
       </c>
       <c r="F317" t="s">
         <v>1917</v>
       </c>
-    </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G317" t="s">
+        <v>2392</v>
+      </c>
+      <c r="K317" t="s">
+        <v>2009</v>
+      </c>
+      <c r="M317" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="318" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>330</v>
       </c>
@@ -16295,14 +16766,23 @@
       <c r="C318" t="s">
         <v>1131</v>
       </c>
+      <c r="D318" t="s">
+        <v>1131</v>
+      </c>
       <c r="E318" t="s">
         <v>1523</v>
       </c>
       <c r="F318" t="s">
         <v>1918</v>
       </c>
-    </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G318" t="s">
+        <v>1918</v>
+      </c>
+      <c r="N318" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="319" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>331</v>
       </c>
@@ -16312,14 +16792,29 @@
       <c r="C319" t="s">
         <v>1132</v>
       </c>
+      <c r="D319" t="s">
+        <v>2393</v>
+      </c>
       <c r="E319" t="s">
         <v>1524</v>
       </c>
       <c r="F319" t="s">
         <v>1919</v>
       </c>
-    </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G319" t="s">
+        <v>2394</v>
+      </c>
+      <c r="H319" t="s">
+        <v>2009</v>
+      </c>
+      <c r="K319" t="s">
+        <v>2009</v>
+      </c>
+      <c r="L319" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="320" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>332</v>
       </c>
@@ -16329,14 +16824,26 @@
       <c r="C320" t="s">
         <v>1133</v>
       </c>
+      <c r="D320" t="s">
+        <v>2395</v>
+      </c>
       <c r="E320" t="s">
         <v>1525</v>
       </c>
       <c r="F320" t="s">
         <v>1920</v>
       </c>
-    </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G320" t="s">
+        <v>2396</v>
+      </c>
+      <c r="K320" t="s">
+        <v>2009</v>
+      </c>
+      <c r="M320" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="321" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>333</v>
       </c>
@@ -16346,14 +16853,23 @@
       <c r="C321" t="s">
         <v>1134</v>
       </c>
+      <c r="D321" t="s">
+        <v>2397</v>
+      </c>
       <c r="E321" t="s">
         <v>1526</v>
       </c>
       <c r="F321" t="s">
         <v>1921</v>
       </c>
-    </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G321" t="s">
+        <v>1921</v>
+      </c>
+      <c r="L321" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="322" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>334</v>
       </c>
@@ -16363,19 +16879,32 @@
       <c r="C322" t="s">
         <v>1135</v>
       </c>
+      <c r="D322" t="s">
+        <v>2398</v>
+      </c>
       <c r="E322" t="s">
         <v>1527</v>
       </c>
       <c r="F322" t="s">
         <v>1922</v>
       </c>
-    </row>
-    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G322" t="s">
+        <v>1922</v>
+      </c>
+      <c r="M322" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="323" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>335</v>
       </c>
-      <c r="B323" t="s">
+      <c r="B323" s="2" t="s">
         <v>743</v>
+      </c>
+      <c r="C323" s="2"/>
+      <c r="D323" t="s">
+        <v>2399</v>
       </c>
       <c r="E323" t="s">
         <v>1528</v>
@@ -16383,8 +16912,20 @@
       <c r="F323" t="s">
         <v>1923</v>
       </c>
-    </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G323" t="s">
+        <v>2400</v>
+      </c>
+      <c r="I323" t="s">
+        <v>2009</v>
+      </c>
+      <c r="J323" t="s">
+        <v>2009</v>
+      </c>
+      <c r="K323" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="324" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>336</v>
       </c>
@@ -16394,14 +16935,26 @@
       <c r="C324" t="s">
         <v>1136</v>
       </c>
+      <c r="D324" t="s">
+        <v>2401</v>
+      </c>
       <c r="E324" t="s">
         <v>1529</v>
       </c>
       <c r="F324" t="s">
         <v>1924</v>
       </c>
-    </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G324" t="s">
+        <v>2402</v>
+      </c>
+      <c r="J324" t="s">
+        <v>2009</v>
+      </c>
+      <c r="M324" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="325" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>337</v>
       </c>
@@ -16411,14 +16964,26 @@
       <c r="C325" t="s">
         <v>1137</v>
       </c>
+      <c r="D325" t="s">
+        <v>2403</v>
+      </c>
       <c r="E325" t="s">
         <v>1530</v>
       </c>
       <c r="F325" t="s">
         <v>1925</v>
       </c>
-    </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G325" t="s">
+        <v>2404</v>
+      </c>
+      <c r="K325" t="s">
+        <v>2009</v>
+      </c>
+      <c r="M325" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="326" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>338</v>
       </c>
@@ -16428,14 +16993,23 @@
       <c r="C326" t="s">
         <v>1138</v>
       </c>
+      <c r="D326" t="s">
+        <v>1138</v>
+      </c>
       <c r="E326" t="s">
         <v>1531</v>
       </c>
       <c r="F326" t="s">
         <v>1926</v>
       </c>
-    </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G326" t="s">
+        <v>1926</v>
+      </c>
+      <c r="N326" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="327" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>339</v>
       </c>
@@ -16445,14 +17019,29 @@
       <c r="C327" t="s">
         <v>983</v>
       </c>
+      <c r="D327" t="s">
+        <v>2181</v>
+      </c>
       <c r="E327" t="s">
         <v>1532</v>
       </c>
       <c r="F327" t="s">
         <v>1762</v>
       </c>
-    </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G327" t="s">
+        <v>2405</v>
+      </c>
+      <c r="J327" t="s">
+        <v>2009</v>
+      </c>
+      <c r="K327" t="s">
+        <v>2009</v>
+      </c>
+      <c r="M327" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="328" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>340</v>
       </c>
@@ -16462,14 +17051,26 @@
       <c r="C328" t="s">
         <v>1139</v>
       </c>
+      <c r="D328" t="s">
+        <v>2406</v>
+      </c>
       <c r="E328" t="s">
         <v>1533</v>
       </c>
       <c r="F328" t="s">
         <v>1927</v>
       </c>
-    </row>
-    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G328" t="s">
+        <v>2407</v>
+      </c>
+      <c r="K328" t="s">
+        <v>2009</v>
+      </c>
+      <c r="L328" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="329" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>341</v>
       </c>
@@ -16479,14 +17080,26 @@
       <c r="C329" t="s">
         <v>1140</v>
       </c>
+      <c r="D329" t="s">
+        <v>1140</v>
+      </c>
       <c r="E329" t="s">
         <v>1534</v>
       </c>
       <c r="F329" t="s">
         <v>1928</v>
       </c>
-    </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G329" t="s">
+        <v>2408</v>
+      </c>
+      <c r="K329" t="s">
+        <v>2009</v>
+      </c>
+      <c r="N329" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="330" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>342</v>
       </c>
@@ -16496,14 +17109,23 @@
       <c r="C330" t="s">
         <v>1141</v>
       </c>
+      <c r="D330" t="s">
+        <v>2409</v>
+      </c>
       <c r="E330" t="s">
         <v>1535</v>
       </c>
       <c r="F330" t="s">
         <v>1929</v>
       </c>
-    </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G330" t="s">
+        <v>1929</v>
+      </c>
+      <c r="M330" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="331" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>343</v>
       </c>
@@ -16513,14 +17135,29 @@
       <c r="C331" t="s">
         <v>1020</v>
       </c>
+      <c r="D331" t="s">
+        <v>2030</v>
+      </c>
       <c r="E331" t="s">
         <v>1230</v>
       </c>
       <c r="F331" t="s">
         <v>1799</v>
       </c>
-    </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G331" t="s">
+        <v>2224</v>
+      </c>
+      <c r="H331" t="s">
+        <v>2009</v>
+      </c>
+      <c r="K331" t="s">
+        <v>2009</v>
+      </c>
+      <c r="L331" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="332" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>344</v>
       </c>
@@ -16530,14 +17167,23 @@
       <c r="C332" t="s">
         <v>1142</v>
       </c>
+      <c r="D332" t="s">
+        <v>2411</v>
+      </c>
       <c r="E332" t="s">
         <v>1536</v>
       </c>
       <c r="F332" t="s">
         <v>1930</v>
       </c>
-    </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G332" t="s">
+        <v>2410</v>
+      </c>
+      <c r="H332" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="333" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>345</v>
       </c>
@@ -16547,14 +17193,26 @@
       <c r="C333" t="s">
         <v>1143</v>
       </c>
+      <c r="D333" t="s">
+        <v>2412</v>
+      </c>
       <c r="E333" t="s">
         <v>1537</v>
       </c>
       <c r="F333" t="s">
         <v>1931</v>
       </c>
-    </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G333" t="s">
+        <v>1931</v>
+      </c>
+      <c r="H333" t="s">
+        <v>2009</v>
+      </c>
+      <c r="L333" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="334" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>346</v>
       </c>
@@ -16564,14 +17222,23 @@
       <c r="C334" t="s">
         <v>1144</v>
       </c>
+      <c r="D334" t="s">
+        <v>1144</v>
+      </c>
       <c r="E334" t="s">
         <v>1538</v>
       </c>
       <c r="F334" t="s">
         <v>1932</v>
       </c>
-    </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G334" t="s">
+        <v>1932</v>
+      </c>
+      <c r="N334" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="335" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>347</v>
       </c>
@@ -16581,19 +17248,35 @@
       <c r="C335" t="s">
         <v>1145</v>
       </c>
+      <c r="D335" t="s">
+        <v>2413</v>
+      </c>
       <c r="E335" t="s">
         <v>1539</v>
       </c>
       <c r="F335" t="s">
         <v>1933</v>
       </c>
-    </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G335" t="s">
+        <v>2414</v>
+      </c>
+      <c r="K335" t="s">
+        <v>2009</v>
+      </c>
+      <c r="L335" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="336" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>348</v>
       </c>
-      <c r="B336" t="s">
+      <c r="B336" s="2" t="s">
         <v>756</v>
+      </c>
+      <c r="C336" s="2"/>
+      <c r="D336" t="s">
+        <v>2415</v>
       </c>
       <c r="E336" t="s">
         <v>1540</v>
@@ -16601,13 +17284,29 @@
       <c r="F336" t="s">
         <v>1934</v>
       </c>
-    </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G336" t="s">
+        <v>2416</v>
+      </c>
+      <c r="I336" t="s">
+        <v>2009</v>
+      </c>
+      <c r="J336" t="s">
+        <v>2009</v>
+      </c>
+      <c r="K336" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="337" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>349</v>
       </c>
-      <c r="B337" t="s">
+      <c r="B337" s="2" t="s">
         <v>757</v>
+      </c>
+      <c r="C337" s="2"/>
+      <c r="D337" t="s">
+        <v>2418</v>
       </c>
       <c r="E337" t="s">
         <v>1541</v>
@@ -16615,8 +17314,17 @@
       <c r="F337" t="s">
         <v>1935</v>
       </c>
-    </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G337" t="s">
+        <v>2417</v>
+      </c>
+      <c r="J337" t="s">
+        <v>2009</v>
+      </c>
+      <c r="K337" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="338" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>350</v>
       </c>
@@ -16626,14 +17334,26 @@
       <c r="C338" t="s">
         <v>1146</v>
       </c>
+      <c r="D338" t="s">
+        <v>2419</v>
+      </c>
       <c r="E338" t="s">
         <v>1542</v>
       </c>
       <c r="F338" t="s">
         <v>1936</v>
       </c>
-    </row>
-    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G338" t="s">
+        <v>2420</v>
+      </c>
+      <c r="K338" t="s">
+        <v>2009</v>
+      </c>
+      <c r="L338" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="339" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>351</v>
       </c>
@@ -16643,19 +17363,38 @@
       <c r="C339" t="s">
         <v>1147</v>
       </c>
+      <c r="D339" t="s">
+        <v>2421</v>
+      </c>
       <c r="E339" t="s">
         <v>1543</v>
       </c>
       <c r="F339" t="s">
         <v>1937</v>
       </c>
-    </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G339" t="s">
+        <v>2422</v>
+      </c>
+      <c r="K339" t="s">
+        <v>2009</v>
+      </c>
+      <c r="L339" t="s">
+        <v>2009</v>
+      </c>
+      <c r="M339" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="340" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>352</v>
       </c>
-      <c r="B340" t="s">
+      <c r="B340" s="2" t="s">
         <v>760</v>
+      </c>
+      <c r="C340" s="2"/>
+      <c r="D340" t="s">
+        <v>2423</v>
       </c>
       <c r="E340" t="s">
         <v>1544</v>
@@ -16663,8 +17402,17 @@
       <c r="F340" t="s">
         <v>1938</v>
       </c>
-    </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G340" t="s">
+        <v>2424</v>
+      </c>
+      <c r="J340" t="s">
+        <v>2009</v>
+      </c>
+      <c r="K340" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="341" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>353</v>
       </c>
@@ -16674,14 +17422,29 @@
       <c r="C341" t="s">
         <v>1148</v>
       </c>
+      <c r="D341" t="s">
+        <v>2425</v>
+      </c>
       <c r="E341" t="s">
         <v>1545</v>
       </c>
       <c r="F341" t="s">
         <v>1939</v>
       </c>
-    </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G341" t="s">
+        <v>2426</v>
+      </c>
+      <c r="K341" t="s">
+        <v>2009</v>
+      </c>
+      <c r="L341" t="s">
+        <v>2009</v>
+      </c>
+      <c r="M341" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="342" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>354</v>
       </c>
@@ -16691,14 +17454,29 @@
       <c r="C342" t="s">
         <v>1149</v>
       </c>
+      <c r="D342" t="s">
+        <v>2427</v>
+      </c>
       <c r="E342" t="s">
         <v>1546</v>
       </c>
       <c r="F342" t="s">
         <v>1940</v>
       </c>
-    </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G342" t="s">
+        <v>2428</v>
+      </c>
+      <c r="I342" t="s">
+        <v>2009</v>
+      </c>
+      <c r="J342" t="s">
+        <v>2009</v>
+      </c>
+      <c r="K342" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="343" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>355</v>
       </c>
@@ -16708,14 +17486,26 @@
       <c r="C343" t="s">
         <v>1150</v>
       </c>
+      <c r="D343" t="s">
+        <v>2429</v>
+      </c>
       <c r="E343" t="s">
         <v>1547</v>
       </c>
       <c r="F343" t="s">
         <v>1941</v>
       </c>
-    </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G343" t="s">
+        <v>2430</v>
+      </c>
+      <c r="K343" t="s">
+        <v>2009</v>
+      </c>
+      <c r="M343" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="344" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>356</v>
       </c>
@@ -16725,19 +17515,32 @@
       <c r="C344" t="s">
         <v>1151</v>
       </c>
+      <c r="D344" t="s">
+        <v>1151</v>
+      </c>
       <c r="E344" t="s">
         <v>1548</v>
       </c>
       <c r="F344" t="s">
         <v>1942</v>
       </c>
-    </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G344" t="s">
+        <v>1942</v>
+      </c>
+      <c r="N344" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="345" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>357</v>
       </c>
-      <c r="B345" t="s">
+      <c r="B345" s="2" t="s">
         <v>765</v>
+      </c>
+      <c r="C345" s="2"/>
+      <c r="D345" t="s">
+        <v>2432</v>
       </c>
       <c r="E345" t="s">
         <v>1549</v>
@@ -16745,8 +17548,17 @@
       <c r="F345" t="s">
         <v>1943</v>
       </c>
-    </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G345" t="s">
+        <v>2431</v>
+      </c>
+      <c r="J345" t="s">
+        <v>2009</v>
+      </c>
+      <c r="K345" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="346" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>358</v>
       </c>
@@ -16756,14 +17568,29 @@
       <c r="C346" t="s">
         <v>1152</v>
       </c>
+      <c r="D346" t="s">
+        <v>2433</v>
+      </c>
       <c r="E346" t="s">
         <v>1550</v>
       </c>
       <c r="F346" t="s">
         <v>1944</v>
       </c>
-    </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G346" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H346" t="s">
+        <v>2009</v>
+      </c>
+      <c r="I346" t="s">
+        <v>2009</v>
+      </c>
+      <c r="K346" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="347" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>359</v>
       </c>
@@ -16777,7 +17604,7 @@
         <v>1945</v>
       </c>
     </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>360</v>
       </c>
@@ -16794,7 +17621,7 @@
         <v>1946</v>
       </c>
     </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>361</v>
       </c>
@@ -16811,7 +17638,7 @@
         <v>1947</v>
       </c>
     </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>362</v>
       </c>
@@ -16828,7 +17655,7 @@
         <v>1948</v>
       </c>
     </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>363</v>
       </c>
@@ -16845,7 +17672,7 @@
         <v>1949</v>
       </c>
     </row>
-    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>364</v>
       </c>

</xml_diff>

<commit_message>
test set translations generated
</commit_message>
<xml_diff>
--- a/Review files/qald9_train_set_review_table.xlsx
+++ b/Review files/qald9_train_set_review_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javi\Desktop\Work\QALD9ES\Repo\QALD9-ES\Review files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9728A7-B407-4EED-B394-D46B6C5146FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F02073-4CE7-4771-A28D-9CE1D115FBB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7996,10 +7996,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+      <selection pane="bottomLeft" activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>